<commit_message>
the notebook and a supposed de-anonymised csv
</commit_message>
<xml_diff>
--- a/Part_2/public_data_resultsE.xlsx
+++ b/Part_2/public_data_resultsE.xlsx
@@ -1,55 +1,62 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <workbookPr date1904="false"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11110"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chris/Desktop/ITU/5thsem/SP/FinalProject/SP_project2024/Part_2/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D89E3EE3-76C4-1D4B-8457-3DDE2B65426D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="13125" windowHeight="6105" firstSheet="0" activeTab="0"/>
+    <workbookView xWindow="0" yWindow="740" windowWidth="13120" windowHeight="17120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet 1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet 1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
-  <si>
-    <t xml:space="preserve"/>
-  </si>
-  <si>
-    <t xml:space="preserve">Red</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Green</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Invalid ballots</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Total</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Polling station: ZIP 2100</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Polling station: ZIP 2200</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Polling station: ZIP 2300</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Polling station: ZIP 2400</t>
-  </si>
-  <si>
-    <t xml:space="preserve">E-votes</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="10">
+  <si>
+    <t>Red</t>
+  </si>
+  <si>
+    <t>Green</t>
+  </si>
+  <si>
+    <t>Invalid ballots</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
+  <si>
+    <t>Polling station: ZIP 2100</t>
+  </si>
+  <si>
+    <t>Polling station: ZIP 2200</t>
+  </si>
+  <si>
+    <t>Polling station: ZIP 2300</t>
+  </si>
+  <si>
+    <t>Polling station: ZIP 2400</t>
+  </si>
+  <si>
+    <t>E-votes</t>
+  </si>
+  <si>
+    <t>zip</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="0"/>
-  <fonts count="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -85,6 +92,15 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -366,139 +382,151 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:E7"/>
   <sheetViews>
-    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="true"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="21.33203125" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
         <v>4</v>
       </c>
+      <c r="B2">
+        <v>32</v>
+      </c>
+      <c r="C2">
+        <v>86</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="E2">
+        <v>119</v>
+      </c>
     </row>
-    <row r="2">
-      <c r="A2" t="s">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
         <v>5</v>
       </c>
-      <c r="B2" t="n">
-        <v>32</v>
-      </c>
-      <c r="C2" t="n">
-        <v>86</v>
-      </c>
-      <c r="D2" t="n">
+      <c r="B3">
+        <v>58</v>
+      </c>
+      <c r="C3">
+        <v>138</v>
+      </c>
+      <c r="D3">
+        <v>5</v>
+      </c>
+      <c r="E3">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4">
+        <v>105</v>
+      </c>
+      <c r="C4">
+        <v>105</v>
+      </c>
+      <c r="D4">
+        <v>5</v>
+      </c>
+      <c r="E4">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5">
+        <v>78</v>
+      </c>
+      <c r="C5">
+        <v>146</v>
+      </c>
+      <c r="D5">
         <v>1</v>
       </c>
-      <c r="E2" t="n">
-        <v>119</v>
+      <c r="E5">
+        <v>225</v>
       </c>
     </row>
-    <row r="3">
-      <c r="A3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" t="n">
-        <v>58</v>
-      </c>
-      <c r="C3" t="n">
-        <v>138</v>
-      </c>
-      <c r="D3" t="n">
-        <v>5</v>
-      </c>
-      <c r="E3" t="n">
-        <v>201</v>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6">
+        <v>108</v>
+      </c>
+      <c r="C6">
+        <v>219</v>
+      </c>
+      <c r="D6">
+        <v>8</v>
+      </c>
+      <c r="E6">
+        <v>335</v>
       </c>
     </row>
-    <row r="4">
-      <c r="A4" t="s">
-        <v>7</v>
-      </c>
-      <c r="B4" t="n">
-        <v>105</v>
-      </c>
-      <c r="C4" t="n">
-        <v>105</v>
-      </c>
-      <c r="D4" t="n">
-        <v>5</v>
-      </c>
-      <c r="E4" t="n">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="s">
-        <v>8</v>
-      </c>
-      <c r="B5" t="n">
-        <v>78</v>
-      </c>
-      <c r="C5" t="n">
-        <v>146</v>
-      </c>
-      <c r="D5" t="n">
-        <v>1</v>
-      </c>
-      <c r="E5" t="n">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="s">
-        <v>9</v>
-      </c>
-      <c r="B6" t="n">
-        <v>108</v>
-      </c>
-      <c r="C6" t="n">
-        <v>219</v>
-      </c>
-      <c r="D6" t="n">
-        <v>8</v>
-      </c>
-      <c r="E6" t="n">
-        <v>335</v>
-      </c>
-    </row>
-    <row r="7">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>4</v>
-      </c>
-      <c r="B7" t="n">
+        <v>3</v>
+      </c>
+      <c r="B7">
         <v>381</v>
       </c>
-      <c r="C7" t="n">
+      <c r="C7">
         <v>694</v>
       </c>
-      <c r="D7" t="n">
+      <c r="D7">
         <v>20</v>
       </c>
-      <c r="E7" t="n">
+      <c r="E7">
         <v>1095</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100EFF4F8DD4AF95548A29E5B36B9FF92C8" ma:contentTypeVersion="4" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="28c60d39cb0c39ba04b38939bb19211e">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="7f72b764-4b0f-4352-b2a3-29d337326309" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="9fce6d31eb3e26b3bf40c8966e532e79" ns2:_="">
     <xsd:import namespace="7f72b764-4b0f-4352-b2a3-29d337326309"/>
@@ -642,15 +670,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement/>
@@ -658,13 +677,36 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{79ACD5DD-B907-4441-860C-4CF2AB7062C4}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6D615EF4-79B5-483F-BA4A-07170CADE5D6}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6D615EF4-79B5-483F-BA4A-07170CADE5D6}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{79ACD5DD-B907-4441-860C-4CF2AB7062C4}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="7f72b764-4b0f-4352-b2a3-29d337326309"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B4222932-88E1-4623-8C8A-EF4D724805E6}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B4222932-88E1-4623-8C8A-EF4D724805E6}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>